<commit_message>
added function to highlight all bars of given country
</commit_message>
<xml_diff>
--- a/conflicts.xlsx
+++ b/conflicts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17660" windowHeight="18000"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="17660" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="conflicts.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="548">
   <si>
     <t>Yemen</t>
   </si>
@@ -988,12 +988,6 @@
   </si>
   <si>
     <t>"Since 1979" may be better, since the end date is indefinite.</t>
-  </si>
-  <si>
-    <t>Other questions</t>
-  </si>
-  <si>
-    <t>If there is more than 1000 state executions per year, would that also count as mass killing? (China)</t>
   </si>
   <si>
     <t>* Numbers seem to include famine deaths. What to do about famine deaths? Some include and others exclude famine deaths.</t>
@@ -3663,9 +3657,6 @@
   </si>
   <si>
     <t>South Asia</t>
-  </si>
-  <si>
-    <t>MISSING</t>
   </si>
   <si>
     <t>Bulgaria</t>
@@ -4030,7 +4021,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4064,12 +4055,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4186,7 +4171,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4399,18 +4384,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4426,16 +4402,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4787,16 +4763,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O130"/>
+  <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:XFD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="76" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="71" customWidth="1"/>
     <col min="3" max="4" width="18.33203125" style="65" customWidth="1"/>
     <col min="5" max="6" width="6.33203125" style="7" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" style="56" customWidth="1"/>
@@ -4812,63 +4788,63 @@
   <sheetData>
     <row r="1" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>473</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>475</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="G1" s="51" t="s">
         <v>463</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="51" t="s">
         <v>464</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>465</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>466</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>467</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>308</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="O1" s="16" t="s">
         <v>470</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>483</v>
-      </c>
-      <c r="B2" s="71" t="s">
-        <v>484</v>
+        <v>480</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>481</v>
       </c>
       <c r="C2" s="62">
         <v>355</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E2" s="18">
         <v>1944</v>
@@ -4887,7 +4863,7 @@
         <v>55138</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>81</v>
@@ -4900,21 +4876,21 @@
       </c>
       <c r="N2" s="20"/>
       <c r="O2" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="B3" s="71" t="s">
-        <v>486</v>
+        <v>482</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>483</v>
       </c>
       <c r="C3" s="62">
         <v>339</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E3" s="18">
         <v>1944</v>
@@ -4933,7 +4909,7 @@
         <v>7500</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>81</v>
@@ -4946,21 +4922,21 @@
       </c>
       <c r="N3" s="24"/>
       <c r="O3" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>487</v>
-      </c>
-      <c r="B4" s="71" t="s">
-        <v>486</v>
+        <v>484</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>483</v>
       </c>
       <c r="C4" s="62">
         <v>290</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E4" s="18">
         <v>1945</v>
@@ -4979,7 +4955,7 @@
         <v>19334</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>81</v>
@@ -4992,21 +4968,21 @@
       </c>
       <c r="N4" s="23"/>
       <c r="O4" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>488</v>
-      </c>
-      <c r="B5" s="71" t="s">
-        <v>484</v>
+        <v>485</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>481</v>
       </c>
       <c r="C5" s="62">
         <v>310</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E5" s="18">
         <v>1945</v>
@@ -5025,7 +5001,7 @@
         <v>2000</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>81</v>
@@ -5038,21 +5014,21 @@
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>489</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>490</v>
+        <v>486</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>487</v>
       </c>
       <c r="C6" s="27">
         <v>345</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E6" s="27">
         <v>1945</v>
@@ -5071,7 +5047,7 @@
         <v>57177.5</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K6" s="29" t="s">
         <v>82</v>
@@ -5084,21 +5060,21 @@
       </c>
       <c r="N6" s="23"/>
       <c r="O6" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>489</v>
-      </c>
-      <c r="B7" s="71" t="s">
-        <v>484</v>
+        <v>486</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>481</v>
       </c>
       <c r="C7" s="27">
         <v>345</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E7" s="31">
         <v>1945</v>
@@ -5117,7 +5093,7 @@
         <v>50000</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>83</v>
@@ -5130,21 +5106,21 @@
       </c>
       <c r="N7" s="23"/>
       <c r="O7" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="77" t="s">
-        <v>484</v>
+      <c r="B8" s="72" t="s">
+        <v>481</v>
       </c>
       <c r="C8" s="62">
         <v>360</v>
       </c>
       <c r="D8" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E8" s="18">
         <v>1945</v>
@@ -5163,7 +5139,7 @@
         <v>230000</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>81</v>
@@ -5176,21 +5152,21 @@
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>490</v>
+        <v>489</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>487</v>
       </c>
       <c r="C9" s="27">
         <v>315</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E9" s="27">
         <v>1945</v>
@@ -5209,7 +5185,7 @@
         <v>24500</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K9" s="29" t="s">
         <v>84</v>
@@ -5222,21 +5198,21 @@
       </c>
       <c r="N9" s="23"/>
       <c r="O9" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="B10" s="69" t="s">
         <v>487</v>
-      </c>
-      <c r="B10" s="72" t="s">
-        <v>490</v>
       </c>
       <c r="C10" s="27">
         <v>290</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E10" s="27">
         <v>1945</v>
@@ -5255,7 +5231,7 @@
         <v>1421700</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K10" s="29" t="s">
         <v>85</v>
@@ -5268,21 +5244,21 @@
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>487</v>
-      </c>
-      <c r="B11" s="72" t="s">
-        <v>493</v>
+        <v>484</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>490</v>
       </c>
       <c r="C11" s="27">
         <v>290</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E11" s="27">
         <v>1945</v>
@@ -5301,7 +5277,7 @@
         <v>5000</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="K11" s="29" t="s">
         <v>86</v>
@@ -5314,21 +5290,21 @@
       </c>
       <c r="N11" s="23"/>
       <c r="O11" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="B12" s="73" t="s">
-        <v>495</v>
+        <v>491</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>492</v>
       </c>
       <c r="C12" s="63">
         <v>840</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E12" s="33">
         <v>1946</v>
@@ -5347,7 +5323,7 @@
         <v>2000</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K12" s="28" t="s">
         <v>87</v>
@@ -5360,21 +5336,21 @@
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>496</v>
-      </c>
-      <c r="B13" s="73" t="s">
-        <v>497</v>
+        <v>493</v>
+      </c>
+      <c r="B13" s="70" t="s">
+        <v>494</v>
       </c>
       <c r="C13" s="63">
         <v>710</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E13" s="33">
         <v>1947</v>
@@ -5393,7 +5369,7 @@
         <v>22500</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K13" s="29" t="s">
         <v>88</v>
@@ -5405,24 +5381,24 @@
         <v>199</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>492</v>
-      </c>
-      <c r="B14" s="73" t="s">
-        <v>498</v>
+        <v>489</v>
+      </c>
+      <c r="B14" s="70" t="s">
+        <v>495</v>
       </c>
       <c r="C14" s="63">
         <v>315</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E14" s="33">
         <v>1948</v>
@@ -5441,7 +5417,7 @@
         <v>18030</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>81</v>
@@ -5454,21 +5430,21 @@
       </c>
       <c r="N14" s="23"/>
       <c r="O14" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>500</v>
-      </c>
-      <c r="B15" s="73" t="s">
-        <v>499</v>
+        <v>497</v>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>496</v>
       </c>
       <c r="C15" s="63">
         <v>775</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E15" s="33">
         <v>1948</v>
@@ -5487,7 +5463,7 @@
         <v>100000</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K15" s="28" t="s">
         <v>89</v>
@@ -5499,24 +5475,24 @@
         <v>197</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>503</v>
-      </c>
-      <c r="B16" s="73" t="s">
-        <v>502</v>
+        <v>500</v>
+      </c>
+      <c r="B16" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="C16" s="63">
         <v>732</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E16" s="33">
         <v>1948</v>
@@ -5535,7 +5511,7 @@
         <v>21362.5</v>
       </c>
       <c r="J16" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K16" s="28" t="s">
         <v>90</v>
@@ -5547,24 +5523,24 @@
         <v>197</v>
       </c>
       <c r="N16" s="23" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="B17" s="73" t="s">
-        <v>505</v>
+        <v>501</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>502</v>
       </c>
       <c r="C17" s="63">
         <v>100</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E17" s="33">
         <v>1948</v>
@@ -5583,7 +5559,7 @@
         <v>100000</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K17" s="28" t="s">
         <v>91</v>
@@ -5596,21 +5572,21 @@
       </c>
       <c r="N17" s="23"/>
       <c r="O17" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>500</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>506</v>
+        <v>497</v>
+      </c>
+      <c r="B18" s="70" t="s">
+        <v>503</v>
       </c>
       <c r="C18" s="63">
         <v>775</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E18" s="33">
         <v>1948</v>
@@ -5629,7 +5605,7 @@
         <v>145000</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K18" s="28" t="s">
         <v>92</v>
@@ -5641,24 +5617,24 @@
         <v>199</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>508</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>484</v>
+        <v>505</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>481</v>
       </c>
       <c r="C19" s="63">
         <v>731</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E19" s="33">
         <v>1948</v>
@@ -5677,7 +5653,7 @@
         <v>950000</v>
       </c>
       <c r="J19" s="34" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>81</v>
@@ -5689,24 +5665,24 @@
         <v>197</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>509</v>
-      </c>
-      <c r="B20" s="73" t="s">
-        <v>510</v>
+        <v>506</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>507</v>
       </c>
       <c r="C20" s="63">
         <v>850</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E20" s="33">
         <v>1949</v>
@@ -5725,7 +5701,7 @@
         <v>2750</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K20" s="28" t="s">
         <v>93</v>
@@ -5738,21 +5714,21 @@
       </c>
       <c r="N20" s="23"/>
       <c r="O20" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="266.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>496</v>
-      </c>
-      <c r="B21" s="73" t="s">
-        <v>511</v>
+        <v>493</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>508</v>
       </c>
       <c r="C21" s="63">
         <v>710</v>
       </c>
       <c r="D21" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E21" s="33">
         <v>1949</v>
@@ -5771,7 +5747,7 @@
         <v>35500000</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K21" s="29" t="s">
         <v>81</v>
@@ -5784,21 +5760,21 @@
       </c>
       <c r="N21" s="23"/>
       <c r="O21" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>512</v>
-      </c>
-      <c r="B22" s="71" t="s">
-        <v>513</v>
+        <v>509</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>510</v>
       </c>
       <c r="C22" s="62">
         <v>90</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E22" s="33">
         <v>1954</v>
@@ -5817,7 +5793,7 @@
         <v>7500</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K22" s="29" t="s">
         <v>94</v>
@@ -5829,24 +5805,24 @@
         <v>211</v>
       </c>
       <c r="N22" s="23" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="72" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>515</v>
-      </c>
-      <c r="B23" s="73" t="s">
-        <v>514</v>
+        <v>512</v>
+      </c>
+      <c r="B23" s="70" t="s">
+        <v>511</v>
       </c>
       <c r="C23" s="63">
         <v>816</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E23" s="33">
         <v>1954</v>
@@ -5865,7 +5841,7 @@
         <v>41000</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K23" s="29" t="s">
         <v>81</v>
@@ -5877,24 +5853,24 @@
         <v>197</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>517</v>
-      </c>
-      <c r="B24" s="71" t="s">
-        <v>518</v>
+        <v>514</v>
+      </c>
+      <c r="B24" s="68" t="s">
+        <v>515</v>
       </c>
       <c r="C24" s="62">
         <v>816</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E24" s="18">
         <v>1954</v>
@@ -5913,7 +5889,7 @@
         <v>225000</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>95</v>
@@ -5925,24 +5901,24 @@
         <v>197</v>
       </c>
       <c r="N24" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="B25" s="71" t="s">
-        <v>520</v>
+        <v>493</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>517</v>
       </c>
       <c r="C25" s="62">
         <v>710</v>
       </c>
       <c r="D25" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E25" s="18">
         <v>1954</v>
@@ -5961,7 +5937,7 @@
         <v>375000</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>96</v>
@@ -5973,24 +5949,24 @@
         <v>201</v>
       </c>
       <c r="N25" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="71" t="s">
-        <v>518</v>
+      <c r="B26" s="68" t="s">
+        <v>515</v>
       </c>
       <c r="C26" s="62">
         <v>625</v>
       </c>
       <c r="D26" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E26" s="18">
         <v>1955</v>
@@ -6009,7 +5985,7 @@
         <v>500000</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>97</v>
@@ -6022,21 +5998,21 @@
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>523</v>
-      </c>
-      <c r="B27" s="71" t="s">
-        <v>524</v>
+        <v>520</v>
+      </c>
+      <c r="B27" s="68" t="s">
+        <v>521</v>
       </c>
       <c r="C27" s="62">
         <v>41</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E27" s="18">
         <v>1958</v>
@@ -6055,7 +6031,7 @@
         <v>35000</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>98</v>
@@ -6068,21 +6044,21 @@
       </c>
       <c r="N27" s="23"/>
       <c r="O27" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B28" s="73" t="s">
-        <v>526</v>
+        <v>522</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>523</v>
       </c>
       <c r="C28" s="63">
         <v>40</v>
       </c>
       <c r="D28" s="63" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E28" s="33">
         <v>1959</v>
@@ -6101,7 +6077,7 @@
         <v>6667.5</v>
       </c>
       <c r="J28" s="34" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K28" s="28" t="s">
         <v>99</v>
@@ -6114,21 +6090,21 @@
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>527</v>
-      </c>
-      <c r="B29" s="73" t="s">
-        <v>528</v>
+        <v>524</v>
+      </c>
+      <c r="B29" s="70" t="s">
+        <v>525</v>
       </c>
       <c r="C29" s="63">
         <v>645</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E29" s="33">
         <v>1959</v>
@@ -6147,7 +6123,7 @@
         <v>1000</v>
       </c>
       <c r="J29" s="34" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K29" s="28" t="s">
         <v>100</v>
@@ -6160,21 +6136,21 @@
       </c>
       <c r="N29" s="23"/>
       <c r="O29" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="72" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>529</v>
-      </c>
-      <c r="B30" s="71" t="s">
-        <v>530</v>
+        <v>526</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>527</v>
       </c>
       <c r="C30" s="62">
         <v>438</v>
       </c>
-      <c r="D30" s="66" t="s">
-        <v>482</v>
+      <c r="D30" s="62" t="s">
+        <v>477</v>
       </c>
       <c r="E30" s="18">
         <v>1960</v>
@@ -6193,7 +6169,7 @@
         <v>28000</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>98</v>
@@ -6206,21 +6182,21 @@
       </c>
       <c r="N30" s="23"/>
       <c r="O30" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>531</v>
-      </c>
-      <c r="B31" s="73" t="s">
-        <v>532</v>
+        <v>528</v>
+      </c>
+      <c r="B31" s="70" t="s">
+        <v>529</v>
       </c>
       <c r="C31" s="63">
         <v>812</v>
       </c>
       <c r="D31" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E31" s="33">
         <v>1959</v>
@@ -6239,7 +6215,7 @@
         <v>60000</v>
       </c>
       <c r="J31" s="34" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K31" s="28" t="s">
         <v>101</v>
@@ -6254,21 +6230,21 @@
         <v>311</v>
       </c>
       <c r="O31" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="B32" s="73" t="s">
-        <v>534</v>
+        <v>530</v>
+      </c>
+      <c r="B32" s="70" t="s">
+        <v>531</v>
       </c>
       <c r="C32" s="63">
         <v>484</v>
       </c>
       <c r="D32" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E32" s="33">
         <v>1960</v>
@@ -6287,7 +6263,7 @@
         <v>5000</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K32" s="28" t="s">
         <v>102</v>
@@ -6300,21 +6276,21 @@
       </c>
       <c r="N32" s="23"/>
       <c r="O32" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>527</v>
-      </c>
-      <c r="B33" s="71" t="s">
-        <v>535</v>
+        <v>524</v>
+      </c>
+      <c r="B33" s="68" t="s">
+        <v>532</v>
       </c>
       <c r="C33" s="62">
         <v>645</v>
       </c>
-      <c r="D33" s="67" t="s">
-        <v>480</v>
+      <c r="D33" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E33" s="18">
         <v>1961</v>
@@ -6333,7 +6309,7 @@
         <v>160000</v>
       </c>
       <c r="J33" s="25" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>103</v>
@@ -6346,21 +6322,21 @@
       </c>
       <c r="N33" s="23"/>
       <c r="O33" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="B34" s="71" t="s">
-        <v>537</v>
+        <v>533</v>
+      </c>
+      <c r="B34" s="68" t="s">
+        <v>534</v>
       </c>
       <c r="C34" s="62">
         <v>530</v>
       </c>
       <c r="D34" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E34" s="18">
         <v>1961</v>
@@ -6379,7 +6355,7 @@
         <v>190000</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>104</v>
@@ -6392,21 +6368,21 @@
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="72" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>538</v>
-      </c>
-      <c r="B35" s="71" t="s">
-        <v>539</v>
+        <v>535</v>
+      </c>
+      <c r="B35" s="68" t="s">
+        <v>536</v>
       </c>
       <c r="C35" s="62">
         <v>615</v>
       </c>
-      <c r="D35" s="67" t="s">
-        <v>480</v>
+      <c r="D35" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E35" s="18">
         <v>1962</v>
@@ -6425,7 +6401,7 @@
         <v>90000</v>
       </c>
       <c r="J35" s="25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>105</v>
@@ -6438,19 +6414,19 @@
       </c>
       <c r="N35" s="23"/>
       <c r="O35" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="71"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="62">
         <v>679</v>
       </c>
-      <c r="D36" s="67" t="s">
-        <v>480</v>
+      <c r="D36" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E36" s="33">
         <v>1962</v>
@@ -6469,7 +6445,7 @@
         <v>35000</v>
       </c>
       <c r="J36" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>106</v>
@@ -6484,21 +6460,21 @@
         <v>312</v>
       </c>
       <c r="O36" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>527</v>
-      </c>
-      <c r="B37" s="71" t="s">
-        <v>540</v>
+        <v>524</v>
+      </c>
+      <c r="B37" s="68" t="s">
+        <v>537</v>
       </c>
       <c r="C37" s="62">
         <v>645</v>
       </c>
-      <c r="D37" s="67" t="s">
-        <v>480</v>
+      <c r="D37" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E37" s="33">
         <v>1963</v>
@@ -6517,7 +6493,7 @@
         <v>85000</v>
       </c>
       <c r="J37" s="25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K37" s="21" t="s">
         <v>107</v>
@@ -6530,19 +6506,19 @@
       </c>
       <c r="N37" s="23"/>
       <c r="O37" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="71"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="62">
         <v>517</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E38" s="18">
         <v>1963</v>
@@ -6561,7 +6537,7 @@
         <v>16000</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K38" s="21" t="s">
         <v>108</v>
@@ -6574,21 +6550,21 @@
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="72" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>541</v>
-      </c>
-      <c r="B39" s="71" t="s">
-        <v>484</v>
+        <v>538</v>
+      </c>
+      <c r="B39" s="68" t="s">
+        <v>481</v>
       </c>
       <c r="C39" s="62">
         <v>511</v>
       </c>
-      <c r="D39" s="66" t="s">
-        <v>482</v>
+      <c r="D39" s="62" t="s">
+        <v>477</v>
       </c>
       <c r="E39" s="18">
         <v>1964</v>
@@ -6607,7 +6583,7 @@
         <v>4500</v>
       </c>
       <c r="J39" s="25" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>109</v>
@@ -6620,21 +6596,21 @@
       </c>
       <c r="N39" s="23"/>
       <c r="O39" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>533</v>
-      </c>
-      <c r="B40" s="71" t="s">
-        <v>542</v>
+        <v>530</v>
+      </c>
+      <c r="B40" s="68" t="s">
+        <v>539</v>
       </c>
       <c r="C40" s="62">
         <v>484</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E40" s="38">
         <v>1964</v>
@@ -6653,7 +6629,7 @@
         <v>3500</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K40" s="29" t="s">
         <v>110</v>
@@ -6668,21 +6644,21 @@
         <v>313</v>
       </c>
       <c r="O40" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>543</v>
-      </c>
-      <c r="B41" s="71" t="s">
-        <v>484</v>
+        <v>540</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>481</v>
       </c>
       <c r="C41" s="62">
         <v>553</v>
       </c>
       <c r="D41" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E41" s="38">
         <v>1964</v>
@@ -6701,7 +6677,7 @@
         <v>6000</v>
       </c>
       <c r="J41" s="25" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="K41" s="29" t="s">
         <v>111</v>
@@ -6714,21 +6690,21 @@
       </c>
       <c r="N41" s="23"/>
       <c r="O41" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>504</v>
-      </c>
-      <c r="B42" s="71" t="s">
-        <v>544</v>
+        <v>501</v>
+      </c>
+      <c r="B42" s="68" t="s">
+        <v>541</v>
       </c>
       <c r="C42" s="62">
         <v>100</v>
       </c>
-      <c r="D42" s="67" t="s">
-        <v>478</v>
+      <c r="D42" s="66" t="s">
+        <v>476</v>
       </c>
       <c r="E42" s="33">
         <v>1965</v>
@@ -6747,7 +6723,7 @@
         <v>50000</v>
       </c>
       <c r="J42" s="25" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="K42" s="21" t="s">
         <v>112</v>
@@ -6760,21 +6736,21 @@
       </c>
       <c r="N42" s="23"/>
       <c r="O42" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>545</v>
-      </c>
-      <c r="B43" s="71" t="s">
-        <v>546</v>
+        <v>542</v>
+      </c>
+      <c r="B43" s="68" t="s">
+        <v>543</v>
       </c>
       <c r="C43" s="62">
         <v>42</v>
       </c>
-      <c r="D43" s="67" t="s">
-        <v>478</v>
+      <c r="D43" s="66" t="s">
+        <v>476</v>
       </c>
       <c r="E43" s="33">
         <v>1965</v>
@@ -6793,7 +6769,7 @@
         <v>4500</v>
       </c>
       <c r="J43" s="25" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K43" s="29" t="s">
         <v>113</v>
@@ -6806,21 +6782,21 @@
       </c>
       <c r="N43" s="23"/>
       <c r="O43" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>509</v>
-      </c>
-      <c r="B44" s="71" t="s">
-        <v>547</v>
+        <v>506</v>
+      </c>
+      <c r="B44" s="68" t="s">
+        <v>544</v>
       </c>
       <c r="C44" s="62">
         <v>850</v>
       </c>
-      <c r="D44" s="67" t="s">
-        <v>477</v>
+      <c r="D44" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E44" s="18">
         <v>1965</v>
@@ -6839,7 +6815,7 @@
         <v>375000</v>
       </c>
       <c r="J44" s="25" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K44" s="21" t="s">
         <v>114</v>
@@ -6852,19 +6828,19 @@
       </c>
       <c r="N44" s="23"/>
       <c r="O44" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="71"/>
+      <c r="B45" s="68"/>
       <c r="C45" s="62">
         <v>516</v>
       </c>
       <c r="D45" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E45" s="18">
         <v>1965</v>
@@ -6883,7 +6859,7 @@
         <v>150000</v>
       </c>
       <c r="J45" s="25" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K45" s="21" t="s">
         <v>115</v>
@@ -6896,21 +6872,21 @@
       </c>
       <c r="N45" s="23"/>
       <c r="O45" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="168" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>548</v>
-      </c>
-      <c r="B46" s="71" t="s">
-        <v>518</v>
+        <v>545</v>
+      </c>
+      <c r="B46" s="68" t="s">
+        <v>515</v>
       </c>
       <c r="C46" s="62">
         <v>811</v>
       </c>
-      <c r="D46" s="67" t="s">
-        <v>477</v>
+      <c r="D46" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E46" s="33">
         <v>1967</v>
@@ -6929,7 +6905,7 @@
         <v>142500</v>
       </c>
       <c r="J46" s="25" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K46" s="28" t="s">
         <v>116</v>
@@ -6944,21 +6920,21 @@
         <v>314</v>
       </c>
       <c r="O46" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>549</v>
-      </c>
-      <c r="B47" s="71" t="s">
-        <v>550</v>
+        <v>546</v>
+      </c>
+      <c r="B47" s="68" t="s">
+        <v>547</v>
       </c>
       <c r="C47" s="62">
         <v>475</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E47" s="18">
         <v>1967</v>
@@ -6977,7 +6953,7 @@
         <v>1300000</v>
       </c>
       <c r="J47" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="K47" s="21" t="s">
         <v>117</v>
@@ -6990,19 +6966,19 @@
       </c>
       <c r="N47" s="23"/>
       <c r="O47" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="276" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="71"/>
+      <c r="B48" s="68"/>
       <c r="C48" s="62">
         <v>411</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E48" s="18">
         <v>1969</v>
@@ -7021,7 +6997,7 @@
         <v>45000</v>
       </c>
       <c r="J48" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K48" s="21" t="s">
         <v>118</v>
@@ -7034,19 +7010,19 @@
       </c>
       <c r="N48" s="23"/>
       <c r="O48" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="132" x14ac:dyDescent="0.2">
-      <c r="A49" s="68" t="s">
+      <c r="A49" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="74"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="62">
         <v>840</v>
       </c>
-      <c r="D49" s="67" t="s">
-        <v>477</v>
+      <c r="D49" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E49" s="39">
         <v>1969</v>
@@ -7065,7 +7041,7 @@
         <v>6500</v>
       </c>
       <c r="J49" s="40" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K49" s="41" t="s">
         <v>119</v>
@@ -7078,19 +7054,19 @@
       </c>
       <c r="N49" s="23"/>
       <c r="O49" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="96" x14ac:dyDescent="0.2">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="75"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="64">
         <v>850</v>
       </c>
-      <c r="D50" s="67" t="s">
-        <v>477</v>
+      <c r="D50" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E50" s="43">
         <v>1969</v>
@@ -7109,7 +7085,7 @@
         <v>40000</v>
       </c>
       <c r="J50" s="40" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K50" s="41" t="s">
         <v>120</v>
@@ -7122,19 +7098,19 @@
       </c>
       <c r="N50" s="23"/>
       <c r="O50" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="71"/>
+      <c r="B51" s="68"/>
       <c r="C51" s="62">
         <v>663</v>
       </c>
-      <c r="D51" s="67" t="s">
-        <v>480</v>
+      <c r="D51" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E51" s="18">
         <v>1970</v>
@@ -7153,7 +7129,7 @@
         <v>1000</v>
       </c>
       <c r="J51" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K51" s="21" t="s">
         <v>121</v>
@@ -7166,19 +7142,19 @@
       </c>
       <c r="N51" s="23"/>
       <c r="O51" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A52" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="71"/>
+      <c r="B52" s="68"/>
       <c r="C52" s="62">
         <v>500</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E52" s="18">
         <v>1971</v>
@@ -7197,7 +7173,7 @@
         <v>165000</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K52" s="21" t="s">
         <v>122</v>
@@ -7210,19 +7186,19 @@
       </c>
       <c r="N52" s="23"/>
       <c r="O52" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A53" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="71"/>
+      <c r="B53" s="68"/>
       <c r="C53" s="62">
         <v>770</v>
       </c>
       <c r="D53" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E53" s="18">
         <v>1971</v>
@@ -7241,7 +7217,7 @@
         <v>650000</v>
       </c>
       <c r="J53" s="25" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>123</v>
@@ -7254,19 +7230,19 @@
       </c>
       <c r="N53" s="23"/>
       <c r="O53" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="71"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="62">
         <v>780</v>
       </c>
       <c r="D54" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E54" s="33">
         <v>1971</v>
@@ -7285,7 +7261,7 @@
         <v>5000</v>
       </c>
       <c r="J54" s="25" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K54" s="21" t="s">
         <v>124</v>
@@ -7298,19 +7274,19 @@
       </c>
       <c r="N54" s="23"/>
       <c r="O54" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A55" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="71"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="62">
         <v>840</v>
       </c>
-      <c r="D55" s="67" t="s">
-        <v>477</v>
+      <c r="D55" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E55" s="18">
         <v>1972</v>
@@ -7329,7 +7305,7 @@
         <v>45000</v>
       </c>
       <c r="J55" s="25" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K55" s="21" t="s">
         <v>125</v>
@@ -7342,19 +7318,19 @@
       </c>
       <c r="N55" s="23"/>
       <c r="O55" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A56" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="71"/>
+      <c r="B56" s="68"/>
       <c r="C56" s="62">
         <v>552</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E56" s="33">
         <v>1972</v>
@@ -7373,7 +7349,7 @@
         <v>7000</v>
       </c>
       <c r="J56" s="25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K56" s="21" t="s">
         <v>126</v>
@@ -7386,19 +7362,19 @@
       </c>
       <c r="N56" s="23"/>
       <c r="O56" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A57" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="71"/>
+      <c r="B57" s="68"/>
       <c r="C57" s="62">
         <v>770</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E57" s="18">
         <v>1973</v>
@@ -7417,7 +7393,7 @@
         <v>1750</v>
       </c>
       <c r="J57" s="25" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K57" s="21" t="s">
         <v>127</v>
@@ -7430,19 +7406,19 @@
       </c>
       <c r="N57" s="23"/>
       <c r="O57" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="71"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="62">
         <v>155</v>
       </c>
-      <c r="D58" s="67" t="s">
-        <v>478</v>
+      <c r="D58" s="66" t="s">
+        <v>476</v>
       </c>
       <c r="E58" s="18">
         <v>1973</v>
@@ -7461,7 +7437,7 @@
         <v>3200</v>
       </c>
       <c r="J58" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>128</v>
@@ -7474,19 +7450,19 @@
       </c>
       <c r="N58" s="23"/>
       <c r="O58" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="156" x14ac:dyDescent="0.2">
       <c r="A59" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="71"/>
+      <c r="B59" s="68"/>
       <c r="C59" s="62">
         <v>530</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E59" s="18">
         <v>1974</v>
@@ -7505,7 +7481,7 @@
         <v>250000</v>
       </c>
       <c r="J59" s="25" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>129</v>
@@ -7517,22 +7493,22 @@
         <v>197</v>
       </c>
       <c r="N59" s="45" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O59" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A60" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="71"/>
+      <c r="B60" s="68"/>
       <c r="C60" s="62">
         <v>93</v>
       </c>
-      <c r="D60" s="67" t="s">
-        <v>478</v>
+      <c r="D60" s="66" t="s">
+        <v>476</v>
       </c>
       <c r="E60" s="33">
         <v>1974</v>
@@ -7551,7 +7527,7 @@
         <v>7000</v>
       </c>
       <c r="J60" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>130</v>
@@ -7564,19 +7540,19 @@
       </c>
       <c r="N60" s="23"/>
       <c r="O60" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A61" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B61" s="71"/>
+      <c r="B61" s="68"/>
       <c r="C61" s="62">
         <v>812</v>
       </c>
-      <c r="D61" s="67" t="s">
-        <v>477</v>
+      <c r="D61" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E61" s="33">
         <v>1975</v>
@@ -7595,7 +7571,7 @@
         <v>20500</v>
       </c>
       <c r="J61" s="25" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K61" s="29" t="s">
         <v>131</v>
@@ -7608,19 +7584,19 @@
       </c>
       <c r="N61" s="23"/>
       <c r="O61" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A62" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="71"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="62">
         <v>811</v>
       </c>
-      <c r="D62" s="67" t="s">
-        <v>477</v>
+      <c r="D62" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E62" s="38">
         <v>1975</v>
@@ -7639,7 +7615,7 @@
         <v>1500000</v>
       </c>
       <c r="J62" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K62" s="29" t="s">
         <v>132</v>
@@ -7652,19 +7628,19 @@
       </c>
       <c r="N62" s="23"/>
       <c r="O62" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A63" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="71"/>
+      <c r="B63" s="68"/>
       <c r="C63" s="62">
         <v>816</v>
       </c>
-      <c r="D63" s="67" t="s">
-        <v>477</v>
+      <c r="D63" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E63" s="18">
         <v>1975</v>
@@ -7683,7 +7659,7 @@
         <v>82500</v>
       </c>
       <c r="J63" s="23" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K63" s="21" t="s">
         <v>133</v>
@@ -7696,19 +7672,19 @@
       </c>
       <c r="N63" s="23"/>
       <c r="O63" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="156" x14ac:dyDescent="0.2">
       <c r="A64" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="71"/>
+      <c r="B64" s="68"/>
       <c r="C64" s="62">
         <v>541</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E64" s="33">
         <v>1975</v>
@@ -7727,7 +7703,7 @@
         <v>31500</v>
       </c>
       <c r="J64" s="23" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K64" s="21" t="s">
         <v>134</v>
@@ -7742,19 +7718,19 @@
         <v>315</v>
       </c>
       <c r="O64" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="180" x14ac:dyDescent="0.2">
       <c r="A65" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="71"/>
+      <c r="B65" s="68"/>
       <c r="C65" s="62">
         <v>540</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E65" s="18">
         <v>1975</v>
@@ -7773,7 +7749,7 @@
         <v>217500</v>
       </c>
       <c r="J65" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K65" s="21" t="s">
         <v>135</v>
@@ -7786,19 +7762,19 @@
       </c>
       <c r="N65" s="23"/>
       <c r="O65" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="156" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="71"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="62">
         <v>850</v>
       </c>
-      <c r="D66" s="67" t="s">
-        <v>477</v>
+      <c r="D66" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="E66" s="18">
         <v>1975</v>
@@ -7817,7 +7793,7 @@
         <v>115000</v>
       </c>
       <c r="J66" s="46" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K66" s="21" t="s">
         <v>136</v>
@@ -7832,19 +7808,19 @@
         <v>316</v>
       </c>
       <c r="O66" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A67" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B67" s="71"/>
+      <c r="B67" s="68"/>
       <c r="C67" s="62">
         <v>160</v>
       </c>
-      <c r="D67" s="67" t="s">
-        <v>478</v>
+      <c r="D67" s="66" t="s">
+        <v>476</v>
       </c>
       <c r="E67" s="18">
         <v>1976</v>
@@ -7863,7 +7839,7 @@
         <v>19500</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K67" s="21" t="s">
         <v>137</v>
@@ -7876,19 +7852,19 @@
       </c>
       <c r="N67" s="23"/>
       <c r="O67" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A68" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B68" s="73"/>
+      <c r="B68" s="70"/>
       <c r="C68" s="63">
         <v>560</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E68" s="33">
         <v>1976</v>
@@ -7907,7 +7883,7 @@
         <v>2700</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K68" s="48" t="s">
         <v>138</v>
@@ -7920,19 +7896,19 @@
       </c>
       <c r="N68" s="23"/>
       <c r="O68" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A69" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B69" s="71"/>
+      <c r="B69" s="68"/>
       <c r="C69" s="62">
         <v>530</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E69" s="18">
         <v>1977</v>
@@ -7951,7 +7927,7 @@
         <v>50000</v>
       </c>
       <c r="J69" s="23" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K69" s="21" t="s">
         <v>139</v>
@@ -7964,19 +7940,19 @@
       </c>
       <c r="N69" s="23"/>
       <c r="O69" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="180" x14ac:dyDescent="0.2">
       <c r="A70" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="71"/>
+      <c r="B70" s="68"/>
       <c r="C70" s="62">
         <v>92</v>
       </c>
-      <c r="D70" s="67" t="s">
-        <v>478</v>
+      <c r="D70" s="66" t="s">
+        <v>476</v>
       </c>
       <c r="E70" s="38">
         <v>1977</v>
@@ -7995,7 +7971,7 @@
         <v>55000</v>
       </c>
       <c r="J70" s="23" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K70" s="29" t="s">
         <v>140</v>
@@ -8008,19 +7984,19 @@
       </c>
       <c r="N70" s="23"/>
       <c r="O70" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A71" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B71" s="71"/>
+      <c r="B71" s="68"/>
       <c r="C71" s="62">
         <v>630</v>
       </c>
-      <c r="D71" s="67" t="s">
-        <v>480</v>
+      <c r="D71" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E71" s="33">
         <v>1978</v>
@@ -8039,7 +8015,7 @@
         <v>2500</v>
       </c>
       <c r="J71" s="23" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K71" s="21" t="s">
         <v>141</v>
@@ -8052,19 +8028,19 @@
       </c>
       <c r="N71" s="23"/>
       <c r="O71" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="156" x14ac:dyDescent="0.2">
       <c r="A72" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="71"/>
+      <c r="B72" s="68"/>
       <c r="C72" s="62">
         <v>700</v>
       </c>
       <c r="D72" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E72" s="18">
         <v>1978</v>
@@ -8083,7 +8059,7 @@
         <v>1400000</v>
       </c>
       <c r="J72" s="46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K72" s="21" t="s">
         <v>142</v>
@@ -8096,19 +8072,19 @@
       </c>
       <c r="N72" s="23"/>
       <c r="O72" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="192" x14ac:dyDescent="0.2">
       <c r="A73" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="71"/>
+      <c r="B73" s="68"/>
       <c r="C73" s="62">
         <v>630</v>
       </c>
-      <c r="D73" s="67" t="s">
-        <v>480</v>
+      <c r="D73" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E73" s="18">
         <v>1979</v>
@@ -8127,7 +8103,7 @@
         <v>15000</v>
       </c>
       <c r="J73" s="46" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K73" s="21" t="s">
         <v>143</v>
@@ -8142,19 +8118,19 @@
         <v>318</v>
       </c>
       <c r="O73" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="192" x14ac:dyDescent="0.2">
       <c r="A74" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B74" s="71"/>
+      <c r="B74" s="68"/>
       <c r="C74" s="62">
         <v>652</v>
       </c>
-      <c r="D74" s="67" t="s">
-        <v>480</v>
+      <c r="D74" s="66" t="s">
+        <v>478</v>
       </c>
       <c r="E74" s="18">
         <v>1979</v>
@@ -8173,7 +8149,7 @@
         <v>17500</v>
       </c>
       <c r="J74" s="23" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K74" s="48" t="s">
         <v>144</v>
@@ -8185,22 +8161,22 @@
         <v>197</v>
       </c>
       <c r="N74" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="O74" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A75" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B75" s="71"/>
+      <c r="B75" s="68"/>
       <c r="C75" s="62">
         <v>771</v>
       </c>
       <c r="D75" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E75" s="18">
         <v>1980</v>
@@ -8219,7 +8195,7 @@
         <v>2250</v>
       </c>
       <c r="J75" s="23" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K75" s="21" t="s">
         <v>145</v>
@@ -8232,19 +8208,19 @@
       </c>
       <c r="N75" s="23"/>
       <c r="O75" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A76" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="71"/>
+      <c r="B76" s="68"/>
       <c r="C76" s="62">
         <v>475</v>
       </c>
       <c r="D76" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E76" s="33">
         <v>1980</v>
@@ -8263,7 +8239,7 @@
         <v>4100</v>
       </c>
       <c r="J76" s="23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K76" s="21" t="s">
         <v>146</v>
@@ -8276,19 +8252,19 @@
       </c>
       <c r="N76" s="23"/>
       <c r="O76" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A77" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="71"/>
+      <c r="B77" s="68"/>
       <c r="C77" s="62">
         <v>135</v>
       </c>
       <c r="D77" s="62" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E77" s="33">
         <v>1980</v>
@@ -8307,7 +8283,7 @@
         <v>25000</v>
       </c>
       <c r="J77" s="23" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K77" s="48" t="s">
         <v>147</v>
@@ -8320,19 +8296,19 @@
       </c>
       <c r="N77" s="23"/>
       <c r="O77" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A78" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="71"/>
+      <c r="B78" s="68"/>
       <c r="C78" s="62">
         <v>500</v>
       </c>
       <c r="D78" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E78" s="18">
         <v>1981</v>
@@ -8351,7 +8327,7 @@
         <v>250000</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="K78" s="21" t="s">
         <v>148</v>
@@ -8364,19 +8340,19 @@
       </c>
       <c r="N78" s="23"/>
       <c r="O78" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="156" x14ac:dyDescent="0.2">
       <c r="A79" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="71"/>
+      <c r="B79" s="68"/>
       <c r="C79" s="62">
         <v>93</v>
       </c>
       <c r="D79" s="62" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E79" s="33">
         <v>1981</v>
@@ -8395,7 +8371,7 @@
         <v>1500</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="K79" s="48" t="s">
         <v>149</v>
@@ -8408,19 +8384,19 @@
       </c>
       <c r="N79" s="23"/>
       <c r="O79" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A80" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B80" s="71"/>
+      <c r="B80" s="68"/>
       <c r="C80" s="62">
         <v>552</v>
       </c>
       <c r="D80" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E80" s="33">
         <v>1982</v>
@@ -8439,7 +8415,7 @@
         <v>20000</v>
       </c>
       <c r="J80" s="49" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K80" s="48" t="s">
         <v>150</v>
@@ -8452,19 +8428,19 @@
       </c>
       <c r="N80" s="23"/>
       <c r="O80" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A81" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B81" s="71"/>
+      <c r="B81" s="68"/>
       <c r="C81" s="62">
         <v>520</v>
       </c>
       <c r="D81" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E81" s="18">
         <v>1982</v>
@@ -8483,7 +8459,7 @@
         <v>55000</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K81" s="21" t="s">
         <v>151</v>
@@ -8495,22 +8471,22 @@
         <v>201</v>
       </c>
       <c r="N81" s="23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O81" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A82" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B82" s="71"/>
+      <c r="B82" s="68"/>
       <c r="C82" s="62">
         <v>483</v>
       </c>
       <c r="D82" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E82" s="33">
         <v>1982</v>
@@ -8529,7 +8505,7 @@
         <v>26000</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="K82" s="21" t="s">
         <v>152</v>
@@ -8542,19 +8518,19 @@
       </c>
       <c r="N82" s="23"/>
       <c r="O82" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="264" x14ac:dyDescent="0.2">
       <c r="A83" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="B83" s="71"/>
+      <c r="B83" s="68"/>
       <c r="C83" s="62">
         <v>625</v>
       </c>
       <c r="D83" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E83" s="18">
         <v>1983</v>
@@ -8573,7 +8549,7 @@
         <v>1750000</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K83" s="21" t="s">
         <v>153</v>
@@ -8586,19 +8562,19 @@
       </c>
       <c r="N83" s="23"/>
       <c r="O83" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A84" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B84" s="73"/>
+      <c r="B84" s="70"/>
       <c r="C84" s="63">
         <v>780</v>
       </c>
       <c r="D84" s="63" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E84" s="33">
         <v>1983</v>
@@ -8617,7 +8593,7 @@
         <v>16000</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K84" s="48" t="s">
         <v>154</v>
@@ -8630,19 +8606,19 @@
       </c>
       <c r="N84" s="23"/>
       <c r="O84" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="156" x14ac:dyDescent="0.2">
       <c r="A85" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B85" s="71"/>
+      <c r="B85" s="68"/>
       <c r="C85" s="62">
         <v>750</v>
       </c>
       <c r="D85" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E85" s="33">
         <v>1984</v>
@@ -8661,7 +8637,7 @@
         <v>3000</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K85" s="21" t="s">
         <v>155</v>
@@ -8674,19 +8650,19 @@
       </c>
       <c r="N85" s="23"/>
       <c r="O85" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A86" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B86" s="71"/>
+      <c r="B86" s="68"/>
       <c r="C86" s="62">
         <v>640</v>
       </c>
       <c r="D86" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E86" s="33">
         <v>1984</v>
@@ -8705,7 +8681,7 @@
         <v>17500</v>
       </c>
       <c r="J86" s="23" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K86" s="21" t="s">
         <v>156</v>
@@ -8717,22 +8693,22 @@
         <v>199</v>
       </c>
       <c r="N86" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O86" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A87" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B87" s="71"/>
+      <c r="B87" s="68"/>
       <c r="C87" s="62">
         <v>678</v>
       </c>
       <c r="D87" s="62" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E87" s="33">
         <v>1986</v>
@@ -8751,7 +8727,7 @@
         <v>1500</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K87" s="29" t="s">
         <v>157</v>
@@ -8764,19 +8740,19 @@
       </c>
       <c r="N87" s="23"/>
       <c r="O87" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A88" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B88" s="71"/>
+      <c r="B88" s="68"/>
       <c r="C88" s="62">
         <v>500</v>
       </c>
       <c r="D88" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E88" s="33">
         <v>1986</v>
@@ -8795,7 +8771,7 @@
         <v>1500</v>
       </c>
       <c r="J88" s="23" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K88" s="29" t="s">
         <v>158</v>
@@ -8808,19 +8784,19 @@
       </c>
       <c r="N88" s="23"/>
       <c r="O88" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="168" x14ac:dyDescent="0.2">
       <c r="A89" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B89" s="71"/>
+      <c r="B89" s="68"/>
       <c r="C89" s="62">
         <v>775</v>
       </c>
       <c r="D89" s="62" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E89" s="33">
         <v>1988</v>
@@ -8839,7 +8815,7 @@
         <v>3000</v>
       </c>
       <c r="J89" s="50" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K89" s="29" t="s">
         <v>159</v>
@@ -8851,22 +8827,22 @@
         <v>197</v>
       </c>
       <c r="N89" s="23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O89" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A90" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B90" s="71"/>
+      <c r="B90" s="68"/>
       <c r="C90" s="62">
         <v>516</v>
       </c>
       <c r="D90" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E90" s="18">
         <v>1988</v>
@@ -8885,7 +8861,7 @@
         <v>175000</v>
       </c>
       <c r="J90" s="25" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="K90" s="21" t="s">
         <v>160</v>
@@ -8898,19 +8874,19 @@
       </c>
       <c r="N90" s="23"/>
       <c r="O90" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A91" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B91" s="71"/>
+      <c r="B91" s="68"/>
       <c r="C91" s="62">
         <v>910</v>
       </c>
-      <c r="D91" s="66" t="s">
-        <v>482</v>
+      <c r="D91" s="62" t="s">
+        <v>475</v>
       </c>
       <c r="E91" s="33">
         <v>1988</v>
@@ -8929,7 +8905,7 @@
         <v>11250</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="K91" s="29" t="s">
         <v>161</v>
@@ -8942,19 +8918,19 @@
       </c>
       <c r="N91" s="23"/>
       <c r="O91" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B92" s="73"/>
+      <c r="B92" s="70"/>
       <c r="C92" s="63">
         <v>850</v>
       </c>
       <c r="D92" s="63" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E92" s="33">
         <v>1989</v>
@@ -8973,7 +8949,7 @@
         <v>9000</v>
       </c>
       <c r="J92" s="34" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K92" s="21" t="s">
         <v>162</v>
@@ -8986,19 +8962,19 @@
       </c>
       <c r="N92" s="23"/>
       <c r="O92" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A93" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B93" s="71"/>
+      <c r="B93" s="68"/>
       <c r="C93" s="62">
         <v>780</v>
       </c>
       <c r="D93" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E93" s="18">
         <v>1988</v>
@@ -9017,7 +8993,7 @@
         <v>42500</v>
       </c>
       <c r="J93" s="25" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K93" s="21" t="s">
         <v>163</v>
@@ -9030,19 +9006,19 @@
       </c>
       <c r="N93" s="23"/>
       <c r="O93" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A94" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B94" s="73"/>
+      <c r="B94" s="70"/>
       <c r="C94" s="63">
         <v>360</v>
       </c>
       <c r="D94" s="63" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E94" s="33">
         <v>1989</v>
@@ -9061,7 +9037,7 @@
         <v>1000</v>
       </c>
       <c r="J94" s="34" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="K94" s="21" t="s">
         <v>164</v>
@@ -9074,19 +9050,19 @@
       </c>
       <c r="N94" s="23"/>
       <c r="O94" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A95" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="B95" s="71"/>
+      <c r="B95" s="68"/>
       <c r="C95" s="62">
         <v>450</v>
       </c>
       <c r="D95" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E95" s="33">
         <v>1989</v>
@@ -9105,7 +9081,7 @@
         <v>11250</v>
       </c>
       <c r="J95" s="25" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K95" s="21" t="s">
         <v>165</v>
@@ -9118,19 +9094,19 @@
       </c>
       <c r="N95" s="23"/>
       <c r="O95" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A96" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B96" s="71"/>
+      <c r="B96" s="68"/>
       <c r="C96" s="62">
         <v>750</v>
       </c>
       <c r="D96" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E96" s="33">
         <v>1990</v>
@@ -9149,7 +9125,7 @@
         <v>30000</v>
       </c>
       <c r="J96" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K96" s="21" t="s">
         <v>166</v>
@@ -9162,19 +9138,19 @@
       </c>
       <c r="N96" s="23"/>
       <c r="O96" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="97" spans="1:15" ht="168" x14ac:dyDescent="0.2">
       <c r="A97" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B97" s="71"/>
+      <c r="B97" s="68"/>
       <c r="C97" s="62">
         <v>517</v>
       </c>
       <c r="D97" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E97" s="18">
         <v>1990</v>
@@ -9193,7 +9169,7 @@
         <v>650000</v>
       </c>
       <c r="J97" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K97" s="21" t="s">
         <v>167</v>
@@ -9206,19 +9182,19 @@
       </c>
       <c r="N97" s="23"/>
       <c r="O97" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="168" x14ac:dyDescent="0.2">
       <c r="A98" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B98" s="71"/>
+      <c r="B98" s="68"/>
       <c r="C98" s="62">
         <v>475</v>
       </c>
       <c r="D98" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E98" s="18">
         <v>1990</v>
@@ -9237,7 +9213,7 @@
         <v>4500</v>
       </c>
       <c r="J98" s="25" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K98" s="21" t="s">
         <v>168</v>
@@ -9250,19 +9226,19 @@
       </c>
       <c r="N98" s="23"/>
       <c r="O98" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="204" x14ac:dyDescent="0.2">
       <c r="A99" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B99" s="71"/>
+      <c r="B99" s="68"/>
       <c r="C99" s="62">
         <v>750</v>
       </c>
       <c r="D99" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E99" s="18">
         <v>1990</v>
@@ -9281,7 +9257,7 @@
         <v>1000</v>
       </c>
       <c r="J99" s="25" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K99" s="21" t="s">
         <v>169</v>
@@ -9293,22 +9269,22 @@
         <v>199</v>
       </c>
       <c r="N99" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O99" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A100" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B100" s="71"/>
+      <c r="B100" s="68"/>
       <c r="C100" s="62">
         <v>483</v>
       </c>
       <c r="D100" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E100" s="33">
         <v>1991</v>
@@ -9327,7 +9303,7 @@
         <v>1500</v>
       </c>
       <c r="J100" s="25" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K100" s="21" t="s">
         <v>170</v>
@@ -9340,19 +9316,19 @@
       </c>
       <c r="N100" s="23"/>
       <c r="O100" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A101" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B101" s="71"/>
+      <c r="B101" s="68"/>
       <c r="C101" s="62">
         <v>451</v>
       </c>
       <c r="D101" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E101" s="33">
         <v>1991</v>
@@ -9371,7 +9347,7 @@
         <v>4500</v>
       </c>
       <c r="J101" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="K101" s="21" t="s">
         <v>171</v>
@@ -9384,19 +9360,19 @@
       </c>
       <c r="N101" s="23"/>
       <c r="O101" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="102" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A102" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B102" s="71"/>
+      <c r="B102" s="68"/>
       <c r="C102" s="62">
         <v>645</v>
       </c>
       <c r="D102" s="62" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E102" s="18">
         <v>1991</v>
@@ -9415,7 +9391,7 @@
         <v>45000</v>
       </c>
       <c r="J102" s="25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K102" s="21" t="s">
         <v>172</v>
@@ -9428,19 +9404,19 @@
       </c>
       <c r="N102" s="23"/>
       <c r="O102" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="103" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A103" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B103" s="71"/>
+      <c r="B103" s="68"/>
       <c r="C103" s="62">
         <v>345</v>
       </c>
       <c r="D103" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E103" s="33">
         <v>1991</v>
@@ -9459,7 +9435,7 @@
         <v>3500</v>
       </c>
       <c r="J103" s="25" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K103" s="21" t="s">
         <v>173</v>
@@ -9472,19 +9448,19 @@
       </c>
       <c r="N103" s="23"/>
       <c r="O103" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A104" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B104" s="71"/>
+      <c r="B104" s="68"/>
       <c r="C104" s="62">
         <v>615</v>
       </c>
       <c r="D104" s="62" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E104" s="18">
         <v>1991</v>
@@ -9503,7 +9479,7 @@
         <v>37500</v>
       </c>
       <c r="J104" s="25" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K104" s="21" t="s">
         <v>174</v>
@@ -9516,19 +9492,19 @@
       </c>
       <c r="N104" s="23"/>
       <c r="O104" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A105" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B105" s="71"/>
+      <c r="B105" s="68"/>
       <c r="C105" s="62">
         <v>373</v>
       </c>
       <c r="D105" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E105" s="33">
         <v>1991</v>
@@ -9547,7 +9523,7 @@
         <v>1500</v>
       </c>
       <c r="J105" s="25" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K105" s="21" t="s">
         <v>175</v>
@@ -9560,19 +9536,19 @@
       </c>
       <c r="N105" s="23"/>
       <c r="O105" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A106" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B106" s="71"/>
+      <c r="B106" s="68"/>
       <c r="C106" s="62">
         <v>41</v>
       </c>
       <c r="D106" s="62" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E106" s="18">
         <v>1991</v>
@@ -9591,7 +9567,7 @@
         <v>3500</v>
       </c>
       <c r="J106" s="25" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="K106" s="21" t="s">
         <v>176</v>
@@ -9604,19 +9580,19 @@
       </c>
       <c r="N106" s="23"/>
       <c r="O106" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="107" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A107" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B107" s="71"/>
+      <c r="B107" s="68"/>
       <c r="C107" s="62">
         <v>345</v>
       </c>
       <c r="D107" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E107" s="18">
         <v>1992</v>
@@ -9635,7 +9611,7 @@
         <v>145000</v>
       </c>
       <c r="J107" s="25" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="K107" s="21" t="s">
         <v>177</v>
@@ -9648,19 +9624,19 @@
       </c>
       <c r="N107" s="23"/>
       <c r="O107" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A108" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B108" s="71"/>
+      <c r="B108" s="68"/>
       <c r="C108" s="62">
         <v>700</v>
       </c>
       <c r="D108" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E108" s="33">
         <v>1992</v>
@@ -9679,7 +9655,7 @@
         <v>6250</v>
       </c>
       <c r="J108" s="25" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K108" s="21" t="s">
         <v>178</v>
@@ -9692,19 +9668,19 @@
       </c>
       <c r="N108" s="23"/>
       <c r="O108" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A109" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B109" s="71"/>
+      <c r="B109" s="68"/>
       <c r="C109" s="62">
         <v>702</v>
       </c>
       <c r="D109" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E109" s="33">
         <v>1992</v>
@@ -9723,7 +9699,7 @@
         <v>17500</v>
       </c>
       <c r="J109" s="25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K109" s="21" t="s">
         <v>179</v>
@@ -9736,19 +9712,19 @@
       </c>
       <c r="N109" s="23"/>
       <c r="O109" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="110" spans="1:15" ht="84" x14ac:dyDescent="0.2">
       <c r="A110" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B110" s="71"/>
+      <c r="B110" s="68"/>
       <c r="C110" s="62">
         <v>372</v>
       </c>
       <c r="D110" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E110" s="33">
         <v>1992</v>
@@ -9767,7 +9743,7 @@
         <v>2000</v>
       </c>
       <c r="J110" s="25" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K110" s="21" t="s">
         <v>180</v>
@@ -9780,19 +9756,19 @@
       </c>
       <c r="N110" s="23"/>
       <c r="O110" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="111" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A111" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B111" s="71"/>
+      <c r="B111" s="68"/>
       <c r="C111" s="62">
         <v>484</v>
       </c>
       <c r="D111" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E111" s="33">
         <v>1992</v>
@@ -9811,7 +9787,7 @@
         <v>5000</v>
       </c>
       <c r="J111" s="25" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K111" s="29" t="s">
         <v>181</v>
@@ -9824,19 +9800,19 @@
       </c>
       <c r="N111" s="23"/>
       <c r="O111" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="112" spans="1:15" ht="192" x14ac:dyDescent="0.2">
       <c r="A112" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B112" s="71"/>
+      <c r="B112" s="68"/>
       <c r="C112" s="62">
         <v>490</v>
       </c>
       <c r="D112" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E112" s="33">
         <v>1993</v>
@@ -9855,7 +9831,7 @@
         <v>9000</v>
       </c>
       <c r="J112" s="25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K112" s="21" t="s">
         <v>182</v>
@@ -9868,19 +9844,19 @@
       </c>
       <c r="N112" s="23"/>
       <c r="O112" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A113" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B113" s="71"/>
+      <c r="B113" s="68"/>
       <c r="C113" s="62">
         <v>517</v>
       </c>
       <c r="D113" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E113" s="33">
         <v>1994</v>
@@ -9899,7 +9875,7 @@
         <v>13000</v>
       </c>
       <c r="J113" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K113" s="21" t="s">
         <v>183</v>
@@ -9912,19 +9888,19 @@
       </c>
       <c r="N113" s="23"/>
       <c r="O113" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A114" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B114" s="71"/>
+      <c r="B114" s="68"/>
       <c r="C114" s="62">
         <v>365</v>
       </c>
       <c r="D114" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E114" s="33">
         <v>1994</v>
@@ -9943,7 +9919,7 @@
         <v>62500</v>
       </c>
       <c r="J114" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K114" s="21" t="s">
         <v>184</v>
@@ -9956,19 +9932,19 @@
       </c>
       <c r="N114" s="23"/>
       <c r="O114" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:15" ht="144" x14ac:dyDescent="0.2">
       <c r="A115" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B115" s="71"/>
+      <c r="B115" s="68"/>
       <c r="C115" s="62">
         <v>790</v>
       </c>
       <c r="D115" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E115" s="31">
         <v>1995</v>
@@ -9987,7 +9963,7 @@
         <v>7000</v>
       </c>
       <c r="J115" s="25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="K115" s="21" t="s">
         <v>185</v>
@@ -10000,19 +9976,19 @@
       </c>
       <c r="N115" s="23"/>
       <c r="O115" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A116" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="B116" s="71"/>
+      <c r="B116" s="68"/>
       <c r="C116" s="62">
         <v>700</v>
       </c>
       <c r="D116" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E116" s="18">
         <v>1996</v>
@@ -10031,7 +10007,7 @@
         <v>7500</v>
       </c>
       <c r="J116" s="25" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K116" s="21" t="s">
         <v>186</v>
@@ -10044,19 +10020,19 @@
       </c>
       <c r="N116" s="23"/>
       <c r="O116" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="117" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A117" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="B117" s="71"/>
+      <c r="B117" s="68"/>
       <c r="C117" s="62">
         <v>484</v>
       </c>
       <c r="D117" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E117" s="33">
         <v>1997</v>
@@ -10075,7 +10051,7 @@
         <v>4000</v>
       </c>
       <c r="J117" s="25" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="K117" s="29" t="s">
         <v>187</v>
@@ -10088,19 +10064,19 @@
       </c>
       <c r="N117" s="23"/>
       <c r="O117" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A118" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B118" s="71"/>
+      <c r="B118" s="68"/>
       <c r="C118" s="62">
         <v>345</v>
       </c>
       <c r="D118" s="62" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E118" s="18">
         <v>1998</v>
@@ -10119,7 +10095,7 @@
         <v>10000</v>
       </c>
       <c r="J118" s="25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="K118" s="21" t="s">
         <v>188</v>
@@ -10132,19 +10108,19 @@
       </c>
       <c r="N118" s="23"/>
       <c r="O118" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A119" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B119" s="71"/>
+      <c r="B119" s="68"/>
       <c r="C119" s="62">
         <v>490</v>
       </c>
       <c r="D119" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E119" s="33">
         <v>1998</v>
@@ -10163,7 +10139,7 @@
         <v>100000</v>
       </c>
       <c r="J119" s="25" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K119" s="21" t="s">
         <v>189</v>
@@ -10176,19 +10152,19 @@
       </c>
       <c r="N119" s="23"/>
       <c r="O119" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="120" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A120" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B120" s="71"/>
+      <c r="B120" s="68"/>
       <c r="C120" s="62">
         <v>450</v>
       </c>
       <c r="D120" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E120" s="33">
         <v>2000</v>
@@ -10207,7 +10183,7 @@
         <v>1000</v>
       </c>
       <c r="J120" s="25" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K120" s="21" t="s">
         <v>190</v>
@@ -10220,19 +10196,19 @@
       </c>
       <c r="N120" s="23"/>
       <c r="O120" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="121" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A121" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B121" s="71"/>
+      <c r="B121" s="68"/>
       <c r="C121" s="62">
         <v>625</v>
       </c>
       <c r="D121" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E121" s="18">
         <v>2003</v>
@@ -10251,10 +10227,10 @@
         <v>250000</v>
       </c>
       <c r="J121" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K121" s="21" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L121" s="22" t="s">
         <v>301</v>
@@ -10264,19 +10240,19 @@
       </c>
       <c r="N121" s="23"/>
       <c r="O121" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="122" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A122" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B122" s="71"/>
+      <c r="B122" s="68"/>
       <c r="C122" s="62">
         <v>780</v>
       </c>
       <c r="D122" s="62" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E122" s="18">
         <v>2009</v>
@@ -10295,7 +10271,7 @@
         <v>11500</v>
       </c>
       <c r="J122" s="25" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K122" s="21" t="s">
         <v>191</v>
@@ -10308,19 +10284,19 @@
       </c>
       <c r="N122" s="23"/>
       <c r="O122" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="123" spans="1:15" ht="108" x14ac:dyDescent="0.2">
       <c r="A123" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B123" s="71"/>
+      <c r="B123" s="68"/>
       <c r="C123" s="62">
         <v>437</v>
       </c>
-      <c r="D123" s="70" t="s">
-        <v>479</v>
+      <c r="D123" s="67" t="s">
+        <v>477</v>
       </c>
       <c r="E123" s="18">
         <v>2010</v>
@@ -10339,7 +10315,7 @@
         <v>2250</v>
       </c>
       <c r="J123" s="25" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K123" s="21" t="s">
         <v>192</v>
@@ -10352,19 +10328,19 @@
       </c>
       <c r="N123" s="23"/>
       <c r="O123" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="124" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A124" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B124" s="71"/>
+      <c r="B124" s="68"/>
       <c r="C124" s="62">
         <v>620</v>
       </c>
       <c r="D124" s="62" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E124" s="18">
         <v>2011</v>
@@ -10383,7 +10359,7 @@
         <v>1300</v>
       </c>
       <c r="J124" s="25" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K124" s="21" t="s">
         <v>193</v>
@@ -10394,19 +10370,19 @@
       <c r="M124" s="21"/>
       <c r="N124" s="23"/>
       <c r="O124" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="125" spans="1:15" ht="132" x14ac:dyDescent="0.2">
       <c r="A125" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B125" s="71"/>
+      <c r="B125" s="68"/>
       <c r="C125" s="62">
         <v>652</v>
       </c>
       <c r="D125" s="62" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E125" s="18">
         <v>2011</v>
@@ -10425,7 +10401,7 @@
         <v>35250</v>
       </c>
       <c r="J125" s="25" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K125" s="21" t="s">
         <v>194</v>
@@ -10437,22 +10413,22 @@
         <v>197</v>
       </c>
       <c r="N125" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O125" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="126" spans="1:15" ht="120" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B126" s="71"/>
+      <c r="B126" s="68"/>
       <c r="C126" s="62">
         <v>625</v>
       </c>
       <c r="D126" s="62" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E126" s="18">
         <v>2011</v>
@@ -10471,7 +10447,7 @@
         <v>1500</v>
       </c>
       <c r="J126" s="25" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K126" s="21"/>
       <c r="L126" s="22" t="s">
@@ -10480,18 +10456,18 @@
       <c r="M126" s="21"/>
       <c r="N126" s="23"/>
       <c r="O126" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="127" spans="1:15" ht="195" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C127" s="65">
         <v>626</v>
       </c>
       <c r="D127" s="65" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E127" s="8">
         <v>2013</v>
@@ -10501,10 +10477,10 @@
       <c r="H127" s="55"/>
       <c r="I127" s="60"/>
       <c r="J127" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L127" s="5" t="s">
         <v>317</v>
@@ -10513,20 +10489,10 @@
         <v>211</v>
       </c>
       <c r="N127" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O127" s="10" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="129" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N129" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="130" spans="14:14" ht="45" x14ac:dyDescent="0.2">
-      <c r="N130" s="10" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>